<commit_message>
Updated some study guides
</commit_message>
<xml_diff>
--- a/files/temp-work-2.xlsx
+++ b/files/temp-work-2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/coltongearhart/Desktop/exam5/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{978B12F6-3FD7-EA42-AF11-04D85F063D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE694CBA-3530-C749-839C-6080A45C0366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17620" firstSheet="1" activeTab="17" xr2:uid="{BB8505BC-BCB7-B340-A120-C046C43AD7BD}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -1557,7 +1557,7 @@
     <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="169" formatCode="0.0000"/>
-    <numFmt numFmtId="178" formatCode="0.00000"/>
+    <numFmt numFmtId="170" formatCode="0.00000"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -1717,7 +1717,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="169">
+  <cellXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1899,57 +1899,16 @@
     <xf numFmtId="6" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1981,9 +1940,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1993,11 +1949,7 @@
     <xf numFmtId="168" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2007,6 +1959,48 @@
     <xf numFmtId="6" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="6" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="6" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2512,13 +2506,13 @@
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B3" s="111">
+      <c r="B3" s="149">
         <v>1</v>
       </c>
-      <c r="C3" s="113">
+      <c r="C3" s="151">
         <v>44927</v>
       </c>
-      <c r="D3" s="113">
+      <c r="D3" s="151">
         <v>45056</v>
       </c>
       <c r="E3" s="52">
@@ -2535,9 +2529,9 @@
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B4" s="111"/>
-      <c r="C4" s="113"/>
-      <c r="D4" s="113"/>
+      <c r="B4" s="149"/>
+      <c r="C4" s="151"/>
+      <c r="D4" s="151"/>
       <c r="E4" s="53">
         <v>45275</v>
       </c>
@@ -2552,9 +2546,9 @@
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B5" s="111"/>
-      <c r="C5" s="113"/>
-      <c r="D5" s="113"/>
+      <c r="B5" s="149"/>
+      <c r="C5" s="151"/>
+      <c r="D5" s="151"/>
       <c r="E5" s="55">
         <v>45289</v>
       </c>
@@ -2566,13 +2560,13 @@
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B6" s="114">
+      <c r="B6" s="152">
         <v>2</v>
       </c>
-      <c r="C6" s="112">
+      <c r="C6" s="150">
         <v>45000</v>
       </c>
-      <c r="D6" s="112">
+      <c r="D6" s="150">
         <v>45038</v>
       </c>
       <c r="E6" s="55">
@@ -2589,9 +2583,9 @@
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B7" s="114"/>
-      <c r="C7" s="112"/>
-      <c r="D7" s="112"/>
+      <c r="B7" s="152"/>
+      <c r="C7" s="150"/>
+      <c r="D7" s="150"/>
       <c r="E7" s="53">
         <v>45148</v>
       </c>
@@ -2603,9 +2597,9 @@
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B8" s="114"/>
-      <c r="C8" s="112"/>
-      <c r="D8" s="112"/>
+      <c r="B8" s="152"/>
+      <c r="C8" s="150"/>
+      <c r="D8" s="150"/>
       <c r="E8" s="55">
         <v>45184</v>
       </c>
@@ -2624,9 +2618,9 @@
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B9" s="114"/>
-      <c r="C9" s="112"/>
-      <c r="D9" s="112"/>
+      <c r="B9" s="152"/>
+      <c r="C9" s="150"/>
+      <c r="D9" s="150"/>
       <c r="E9" s="55">
         <v>45234</v>
       </c>
@@ -2638,13 +2632,13 @@
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B10" s="111">
+      <c r="B10" s="149">
         <v>3</v>
       </c>
-      <c r="C10" s="112">
+      <c r="C10" s="150">
         <v>45048</v>
       </c>
-      <c r="D10" s="112">
+      <c r="D10" s="150">
         <v>45152</v>
       </c>
       <c r="E10" s="55">
@@ -2668,9 +2662,9 @@
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B11" s="111"/>
-      <c r="C11" s="112"/>
-      <c r="D11" s="112"/>
+      <c r="B11" s="149"/>
+      <c r="C11" s="150"/>
+      <c r="D11" s="150"/>
       <c r="E11" s="53">
         <v>45206</v>
       </c>
@@ -2692,9 +2686,9 @@
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B12" s="111"/>
-      <c r="C12" s="112"/>
-      <c r="D12" s="112"/>
+      <c r="B12" s="149"/>
+      <c r="C12" s="150"/>
+      <c r="D12" s="150"/>
       <c r="E12" s="55">
         <v>45281</v>
       </c>
@@ -2836,43 +2830,43 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B2" s="119" t="s">
+      <c r="B2" s="156" t="s">
         <v>278</v>
       </c>
-      <c r="C2" s="119"/>
-      <c r="D2" s="119"/>
-      <c r="E2" s="119"/>
-      <c r="F2" s="119"/>
-      <c r="H2" s="119" t="s">
+      <c r="C2" s="156"/>
+      <c r="D2" s="156"/>
+      <c r="E2" s="156"/>
+      <c r="F2" s="156"/>
+      <c r="H2" s="156" t="s">
         <v>280</v>
       </c>
-      <c r="I2" s="119"/>
-      <c r="J2" s="119"/>
-      <c r="K2" s="119"/>
-      <c r="L2" s="119"/>
+      <c r="I2" s="156"/>
+      <c r="J2" s="156"/>
+      <c r="K2" s="156"/>
+      <c r="L2" s="156"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B3" s="118" t="s">
+      <c r="B3" s="157" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="119" t="s">
+      <c r="C3" s="156" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="119"/>
-      <c r="E3" s="119"/>
-      <c r="F3" s="119"/>
-      <c r="H3" s="118" t="s">
+      <c r="D3" s="156"/>
+      <c r="E3" s="156"/>
+      <c r="F3" s="156"/>
+      <c r="H3" s="157" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="119" t="s">
+      <c r="I3" s="156" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="119"/>
-      <c r="K3" s="119"/>
-      <c r="L3" s="119"/>
+      <c r="J3" s="156"/>
+      <c r="K3" s="156"/>
+      <c r="L3" s="156"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B4" s="118"/>
+      <c r="B4" s="157"/>
       <c r="C4" s="2">
         <v>12</v>
       </c>
@@ -2885,7 +2879,7 @@
       <c r="F4" s="2">
         <v>48</v>
       </c>
-      <c r="H4" s="118"/>
+      <c r="H4" s="157"/>
       <c r="I4" s="79" t="s">
         <v>9</v>
       </c>
@@ -3039,13 +3033,13 @@
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B12" s="119" t="s">
+      <c r="B12" s="156" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="119"/>
-      <c r="D12" s="119"/>
-      <c r="E12" s="119"/>
-      <c r="F12" s="119"/>
+      <c r="C12" s="156"/>
+      <c r="D12" s="156"/>
+      <c r="E12" s="156"/>
+      <c r="F12" s="156"/>
       <c r="H12" s="3" t="s">
         <v>26</v>
       </c>
@@ -3066,22 +3060,22 @@
       </c>
     </row>
     <row r="13" spans="2:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="118" t="s">
+      <c r="B13" s="157" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="119" t="s">
+      <c r="C13" s="156" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="119"/>
-      <c r="E13" s="119"/>
-      <c r="F13" s="119"/>
+      <c r="D13" s="156"/>
+      <c r="E13" s="156"/>
+      <c r="F13" s="156"/>
       <c r="H13" s="3"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B14" s="118"/>
+      <c r="B14" s="157"/>
       <c r="C14" s="2">
         <v>12</v>
       </c>
@@ -3115,13 +3109,13 @@
       <c r="F15" s="15">
         <v>50</v>
       </c>
-      <c r="H15" s="119" t="s">
+      <c r="H15" s="156" t="s">
         <v>281</v>
       </c>
-      <c r="I15" s="119"/>
-      <c r="J15" s="119"/>
-      <c r="K15" s="119"/>
-      <c r="L15" s="119"/>
+      <c r="I15" s="156"/>
+      <c r="J15" s="156"/>
+      <c r="K15" s="156"/>
+      <c r="L15" s="156"/>
     </row>
     <row r="16" spans="2:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="15">
@@ -3137,15 +3131,15 @@
         <v>100</v>
       </c>
       <c r="F16" s="15"/>
-      <c r="H16" s="118" t="s">
+      <c r="H16" s="157" t="s">
         <v>3</v>
       </c>
-      <c r="I16" s="119" t="s">
+      <c r="I16" s="156" t="s">
         <v>20</v>
       </c>
-      <c r="J16" s="119"/>
-      <c r="K16" s="119"/>
-      <c r="L16" s="119"/>
+      <c r="J16" s="156"/>
+      <c r="K16" s="156"/>
+      <c r="L16" s="156"/>
     </row>
     <row r="17" spans="2:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="15">
@@ -3159,7 +3153,7 @@
       </c>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
-      <c r="H17" s="118"/>
+      <c r="H17" s="157"/>
       <c r="I17" s="2">
         <v>12</v>
       </c>
@@ -3282,27 +3276,27 @@
       <c r="K22" s="15"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="H24" s="119" t="s">
+      <c r="H24" s="156" t="s">
         <v>282</v>
       </c>
-      <c r="I24" s="119"/>
-      <c r="J24" s="119"/>
-      <c r="K24" s="119"/>
-      <c r="L24" s="119"/>
+      <c r="I24" s="156"/>
+      <c r="J24" s="156"/>
+      <c r="K24" s="156"/>
+      <c r="L24" s="156"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="H25" s="118" t="s">
+      <c r="H25" s="157" t="s">
         <v>3</v>
       </c>
-      <c r="I25" s="119" t="s">
+      <c r="I25" s="156" t="s">
         <v>20</v>
       </c>
-      <c r="J25" s="119"/>
-      <c r="K25" s="119"/>
-      <c r="L25" s="119"/>
+      <c r="J25" s="156"/>
+      <c r="K25" s="156"/>
+      <c r="L25" s="156"/>
     </row>
     <row r="26" spans="2:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H26" s="118"/>
+      <c r="H26" s="157"/>
       <c r="I26" s="79" t="s">
         <v>9</v>
       </c>
@@ -3447,27 +3441,27 @@
       </c>
     </row>
     <row r="37" spans="8:15" x14ac:dyDescent="0.2">
-      <c r="H37" s="119" t="s">
+      <c r="H37" s="156" t="s">
         <v>283</v>
       </c>
-      <c r="I37" s="119"/>
-      <c r="J37" s="119"/>
-      <c r="K37" s="119"/>
-      <c r="L37" s="119"/>
+      <c r="I37" s="156"/>
+      <c r="J37" s="156"/>
+      <c r="K37" s="156"/>
+      <c r="L37" s="156"/>
     </row>
     <row r="38" spans="8:15" x14ac:dyDescent="0.2">
-      <c r="H38" s="118" t="s">
+      <c r="H38" s="157" t="s">
         <v>3</v>
       </c>
-      <c r="I38" s="119" t="s">
+      <c r="I38" s="156" t="s">
         <v>20</v>
       </c>
-      <c r="J38" s="119"/>
-      <c r="K38" s="119"/>
-      <c r="L38" s="119"/>
+      <c r="J38" s="156"/>
+      <c r="K38" s="156"/>
+      <c r="L38" s="156"/>
     </row>
     <row r="39" spans="8:15" x14ac:dyDescent="0.2">
-      <c r="H39" s="118"/>
+      <c r="H39" s="157"/>
       <c r="I39" s="2">
         <v>12</v>
       </c>
@@ -3615,12 +3609,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="H37:L37"/>
+    <mergeCell ref="H38:H39"/>
+    <mergeCell ref="I38:L38"/>
+    <mergeCell ref="H25:H26"/>
+    <mergeCell ref="I25:L25"/>
     <mergeCell ref="H24:L24"/>
     <mergeCell ref="H15:L15"/>
     <mergeCell ref="H16:H17"/>
@@ -3628,11 +3621,12 @@
     <mergeCell ref="H2:L2"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="I3:L3"/>
-    <mergeCell ref="H37:L37"/>
-    <mergeCell ref="H38:H39"/>
-    <mergeCell ref="I38:L38"/>
-    <mergeCell ref="H25:H26"/>
-    <mergeCell ref="I25:L25"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B12:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3661,10 +3655,10 @@
       <c r="D2" s="7" t="s">
         <v>305</v>
       </c>
-      <c r="E2" s="122" t="s">
+      <c r="E2" s="160" t="s">
         <v>306</v>
       </c>
-      <c r="F2" s="123"/>
+      <c r="F2" s="161"/>
       <c r="G2" s="7" t="s">
         <v>307</v>
       </c>
@@ -3888,30 +3882,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="121" t="s">
+      <c r="B2" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="119" t="s">
+      <c r="C2" s="156" t="s">
         <v>310</v>
       </c>
-      <c r="D2" s="119"/>
-      <c r="E2" s="119"/>
-      <c r="F2" s="119"/>
-      <c r="G2" s="121" t="s">
+      <c r="D2" s="156"/>
+      <c r="E2" s="156"/>
+      <c r="F2" s="156"/>
+      <c r="G2" s="159" t="s">
         <v>311</v>
       </c>
-      <c r="I2" s="121" t="s">
+      <c r="I2" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="119" t="s">
+      <c r="J2" s="156" t="s">
         <v>314</v>
       </c>
-      <c r="K2" s="119"/>
-      <c r="L2" s="119"/>
-      <c r="M2" s="119"/>
+      <c r="K2" s="156"/>
+      <c r="L2" s="156"/>
+      <c r="M2" s="156"/>
     </row>
     <row r="3" spans="2:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="B3" s="121"/>
+      <c r="B3" s="159"/>
       <c r="C3" s="48" t="s">
         <v>318</v>
       </c>
@@ -3924,8 +3918,8 @@
       <c r="F3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="121"/>
-      <c r="I3" s="121"/>
+      <c r="G3" s="159"/>
+      <c r="I3" s="159"/>
       <c r="J3" s="48" t="s">
         <v>318</v>
       </c>
@@ -4050,19 +4044,19 @@
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B9" s="121" t="s">
+      <c r="B9" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="119" t="s">
+      <c r="C9" s="156" t="s">
         <v>313</v>
       </c>
-      <c r="D9" s="119"/>
-      <c r="E9" s="119"/>
-      <c r="F9" s="119"/>
-      <c r="G9" s="125"/>
+      <c r="D9" s="156"/>
+      <c r="E9" s="156"/>
+      <c r="F9" s="156"/>
+      <c r="G9" s="2"/>
     </row>
     <row r="10" spans="2:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="B10" s="121"/>
+      <c r="B10" s="159"/>
       <c r="C10" s="48" t="s">
         <v>318</v>
       </c>
@@ -4172,12 +4166,12 @@
       <c r="I15" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="J15" s="119" t="s">
+      <c r="J15" s="156" t="s">
         <v>316</v>
       </c>
-      <c r="K15" s="119"/>
-      <c r="L15" s="119"/>
-      <c r="M15" s="125"/>
+      <c r="K15" s="156"/>
+      <c r="L15" s="156"/>
+      <c r="M15" s="2"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.2">
       <c r="I16" s="48"/>
@@ -4208,7 +4202,7 @@
         <f>FORECAST($M$12,E11:F11,$L4:$M4)</f>
         <v>10000</v>
       </c>
-      <c r="M17" s="130" t="s">
+      <c r="M17" s="116" t="s">
         <v>328</v>
       </c>
     </row>
@@ -4224,7 +4218,7 @@
         <f>FORECAST($L$12,D12:E12,$K5:$L5)</f>
         <v>7030</v>
       </c>
-      <c r="L18" s="130" t="s">
+      <c r="L18" s="116" t="s">
         <v>327</v>
       </c>
       <c r="M18" s="15"/>
@@ -4237,7 +4231,7 @@
         <f>FORECAST($K$12,C13:D13,$J6:$K6)</f>
         <v>3900</v>
       </c>
-      <c r="K19" s="130" t="s">
+      <c r="K19" s="116" t="s">
         <v>326</v>
       </c>
       <c r="L19" s="15"/>
@@ -4247,11 +4241,11 @@
       <c r="I22" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="J22" s="119" t="s">
+      <c r="J22" s="156" t="s">
         <v>319</v>
       </c>
-      <c r="K22" s="119"/>
-      <c r="L22" s="125"/>
+      <c r="K22" s="156"/>
+      <c r="L22" s="2"/>
     </row>
     <row r="23" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I23" s="48"/>
@@ -4267,15 +4261,15 @@
       <c r="I24" s="15">
         <v>2009</v>
       </c>
-      <c r="J24" s="126">
+      <c r="J24" s="112">
         <f>K17/J17</f>
         <v>2.3028500038487918</v>
       </c>
-      <c r="K24" s="126">
+      <c r="K24" s="112">
         <f>L17/K17</f>
         <v>1.2487371206786617</v>
       </c>
-      <c r="L24" s="129" t="s">
+      <c r="L24" s="115" t="s">
         <v>329</v>
       </c>
     </row>
@@ -4283,16 +4277,16 @@
       <c r="I25" s="15">
         <v>2010</v>
       </c>
-      <c r="J25" s="126">
+      <c r="J25" s="112">
         <f t="shared" ref="J25" si="2">K18/J18</f>
         <v>1.9386997757107305</v>
       </c>
-      <c r="K25" s="126"/>
+      <c r="K25" s="112"/>
       <c r="L25" s="22"/>
     </row>
     <row r="26" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I26" s="15"/>
-      <c r="J26" s="126"/>
+      <c r="J26" s="112"/>
       <c r="K26" s="22"/>
       <c r="L26" s="15"/>
     </row>
@@ -4316,11 +4310,11 @@
       <c r="I29" t="s">
         <v>168</v>
       </c>
-      <c r="J29" s="127">
+      <c r="J29" s="113">
         <f>AVERAGE(J24:J25)</f>
         <v>2.1207748897797609</v>
       </c>
-      <c r="K29" s="127">
+      <c r="K29" s="113">
         <f>AVERAGE(K24:K25)</f>
         <v>1.2487371206786617</v>
       </c>
@@ -4346,16 +4340,16 @@
       </c>
     </row>
     <row r="34" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P34" s="121" t="s">
+      <c r="P34" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="Q34" s="119" t="s">
+      <c r="Q34" s="156" t="s">
         <v>310</v>
       </c>
-      <c r="R34" s="119"/>
-      <c r="S34" s="119"/>
-      <c r="T34" s="119"/>
-      <c r="U34" s="121" t="s">
+      <c r="R34" s="156"/>
+      <c r="S34" s="156"/>
+      <c r="T34" s="156"/>
+      <c r="U34" s="159" t="s">
         <v>311</v>
       </c>
       <c r="W34" t="s">
@@ -4376,7 +4370,7 @@
       </c>
     </row>
     <row r="35" spans="16:28" ht="17" x14ac:dyDescent="0.2">
-      <c r="P35" s="121"/>
+      <c r="P35" s="159"/>
       <c r="Q35" s="48" t="s">
         <v>318</v>
       </c>
@@ -4389,7 +4383,7 @@
       <c r="T35" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="U35" s="121"/>
+      <c r="U35" s="159"/>
       <c r="W35" s="3" t="s">
         <v>315</v>
       </c>
@@ -4466,18 +4460,18 @@
       <c r="U38" s="15">
         <v>901</v>
       </c>
-      <c r="W38" s="121" t="s">
+      <c r="W38" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="X38" s="119" t="s">
+      <c r="X38" s="156" t="s">
         <v>336</v>
       </c>
-      <c r="Y38" s="119"/>
-      <c r="Z38" s="119"/>
-      <c r="AA38" s="119"/>
+      <c r="Y38" s="156"/>
+      <c r="Z38" s="156"/>
+      <c r="AA38" s="156"/>
     </row>
     <row r="39" spans="16:28" ht="17" x14ac:dyDescent="0.2">
-      <c r="W39" s="121"/>
+      <c r="W39" s="159"/>
       <c r="X39" s="48" t="s">
         <v>318</v>
       </c>
@@ -4504,7 +4498,7 @@
         <v>462.40000000000003</v>
       </c>
       <c r="Z40" s="13">
-        <f t="shared" ref="Y40:AA41" si="3">Z$35*$U36</f>
+        <f t="shared" ref="Z40" si="3">Z$35*$U36</f>
         <v>663.85</v>
       </c>
       <c r="AA40" s="13">
@@ -4513,15 +4507,15 @@
       </c>
     </row>
     <row r="41" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P41" s="121" t="s">
+      <c r="P41" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="Q41" s="119" t="s">
+      <c r="Q41" s="156" t="s">
         <v>313</v>
       </c>
-      <c r="R41" s="119"/>
-      <c r="S41" s="119"/>
-      <c r="T41" s="119"/>
+      <c r="R41" s="156"/>
+      <c r="S41" s="156"/>
+      <c r="T41" s="156"/>
       <c r="W41" s="15">
         <v>2010</v>
       </c>
@@ -4542,7 +4536,7 @@
       </c>
     </row>
     <row r="42" spans="16:28" ht="17" x14ac:dyDescent="0.2">
-      <c r="P42" s="121"/>
+      <c r="P42" s="159"/>
       <c r="Q42" s="48" t="s">
         <v>318</v>
       </c>
@@ -4618,30 +4612,30 @@
       </c>
       <c r="S45" s="15"/>
       <c r="T45" s="15"/>
-      <c r="W45" s="132"/>
-      <c r="X45" s="125"/>
-      <c r="Y45" s="133" t="s">
+      <c r="W45" s="118"/>
+      <c r="X45" s="2"/>
+      <c r="Y45" s="42" t="s">
         <v>346</v>
       </c>
-      <c r="Z45" s="133" t="s">
+      <c r="Z45" s="42" t="s">
         <v>347</v>
       </c>
-      <c r="AA45" s="125"/>
+      <c r="AA45" s="2"/>
     </row>
     <row r="46" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="W46" s="121" t="s">
+      <c r="W46" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="X46" s="119" t="s">
+      <c r="X46" s="156" t="s">
         <v>337</v>
       </c>
-      <c r="Y46" s="119"/>
-      <c r="Z46" s="119"/>
-      <c r="AA46" s="119"/>
+      <c r="Y46" s="156"/>
+      <c r="Z46" s="156"/>
+      <c r="AA46" s="156"/>
       <c r="AB46" s="2"/>
     </row>
     <row r="47" spans="16:28" ht="17" x14ac:dyDescent="0.2">
-      <c r="W47" s="121"/>
+      <c r="W47" s="159"/>
       <c r="X47" s="48" t="s">
         <v>318</v>
       </c>
@@ -4657,15 +4651,15 @@
       <c r="AB47" s="4"/>
     </row>
     <row r="48" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P48" s="121" t="s">
+      <c r="P48" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="Q48" s="119" t="s">
+      <c r="Q48" s="156" t="s">
         <v>314</v>
       </c>
-      <c r="R48" s="119"/>
-      <c r="S48" s="119"/>
-      <c r="T48" s="119"/>
+      <c r="R48" s="156"/>
+      <c r="S48" s="156"/>
+      <c r="T48" s="156"/>
       <c r="W48" s="15">
         <v>2009</v>
       </c>
@@ -4685,7 +4679,7 @@
       <c r="AB48" s="4"/>
     </row>
     <row r="49" spans="16:28" ht="17" x14ac:dyDescent="0.2">
-      <c r="P49" s="121"/>
+      <c r="P49" s="159"/>
       <c r="Q49" s="48" t="s">
         <v>318</v>
       </c>
@@ -4776,35 +4770,35 @@
       <c r="T52" s="15"/>
     </row>
     <row r="55" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P55" s="121" t="s">
+      <c r="P55" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="Q55" s="119" t="s">
+      <c r="Q55" s="156" t="s">
         <v>333</v>
       </c>
-      <c r="R55" s="119"/>
-      <c r="S55" s="119"/>
-      <c r="T55" s="119"/>
-      <c r="U55" s="119"/>
-      <c r="V55" s="119"/>
+      <c r="R55" s="156"/>
+      <c r="S55" s="156"/>
+      <c r="T55" s="156"/>
+      <c r="U55" s="156"/>
+      <c r="V55" s="156"/>
     </row>
     <row r="56" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P56" s="121"/>
-      <c r="Q56" s="119" t="s">
+      <c r="P56" s="159"/>
+      <c r="Q56" s="156" t="s">
         <v>4</v>
       </c>
-      <c r="R56" s="119"/>
-      <c r="S56" s="119" t="s">
+      <c r="R56" s="156"/>
+      <c r="S56" s="156" t="s">
         <v>5</v>
       </c>
-      <c r="T56" s="119"/>
-      <c r="U56" s="119" t="s">
+      <c r="T56" s="156"/>
+      <c r="U56" s="156" t="s">
         <v>6</v>
       </c>
-      <c r="V56" s="119"/>
+      <c r="V56" s="156"/>
     </row>
     <row r="57" spans="16:28" x14ac:dyDescent="0.2">
-      <c r="P57" s="121"/>
+      <c r="P57" s="159"/>
       <c r="Q57" s="2" t="s">
         <v>334</v>
       </c>
@@ -4828,16 +4822,16 @@
       <c r="P58" s="15">
         <v>2009</v>
       </c>
-      <c r="S58" s="124">
+      <c r="S58" s="111">
         <v>1392.49</v>
       </c>
-      <c r="T58" s="131">
+      <c r="T58" s="117">
         <v>2.5999999999999999E-3</v>
       </c>
-      <c r="U58" s="124">
+      <c r="U58" s="111">
         <v>4198.5</v>
       </c>
-      <c r="V58" s="131">
+      <c r="V58" s="117">
         <v>1.0200000000000001E-3</v>
       </c>
     </row>
@@ -4845,17 +4839,33 @@
       <c r="P59" s="15">
         <v>2010</v>
       </c>
-      <c r="S59" s="124">
+      <c r="S59" s="111">
         <v>1798.09</v>
       </c>
-      <c r="T59" s="131">
+      <c r="T59" s="117">
         <v>1.97E-3</v>
       </c>
-      <c r="U59" s="124"/>
-      <c r="V59" s="131"/>
+      <c r="U59" s="111"/>
+      <c r="V59" s="117"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="P34:P35"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="Q34:T34"/>
+    <mergeCell ref="U34:U35"/>
+    <mergeCell ref="P41:P42"/>
+    <mergeCell ref="Q41:T41"/>
+    <mergeCell ref="P48:P49"/>
+    <mergeCell ref="Q48:T48"/>
     <mergeCell ref="W38:W39"/>
     <mergeCell ref="X38:AA38"/>
     <mergeCell ref="W46:W47"/>
@@ -4865,22 +4875,6 @@
     <mergeCell ref="S56:T56"/>
     <mergeCell ref="Q56:R56"/>
     <mergeCell ref="Q55:V55"/>
-    <mergeCell ref="Q34:T34"/>
-    <mergeCell ref="U34:U35"/>
-    <mergeCell ref="P41:P42"/>
-    <mergeCell ref="Q41:T41"/>
-    <mergeCell ref="P48:P49"/>
-    <mergeCell ref="Q48:T48"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="J15:L15"/>
-    <mergeCell ref="P34:P35"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="I2:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4902,25 +4896,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B2" s="121" t="s">
+      <c r="B2" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="119" t="s">
+      <c r="C2" s="156" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="119"/>
-      <c r="E2" s="119"/>
-      <c r="G2" s="121" t="s">
+      <c r="D2" s="156"/>
+      <c r="E2" s="156"/>
+      <c r="G2" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="119" t="s">
+      <c r="H2" s="156" t="s">
         <v>349</v>
       </c>
-      <c r="I2" s="119"/>
-      <c r="J2" s="119"/>
+      <c r="I2" s="156"/>
+      <c r="J2" s="156"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B3" s="121"/>
+      <c r="B3" s="159"/>
       <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
@@ -4930,7 +4924,7 @@
       <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="121"/>
+      <c r="G3" s="159"/>
       <c r="H3" s="2" t="s">
         <v>4</v>
       </c>
@@ -4957,15 +4951,15 @@
       <c r="G4" s="15">
         <v>2009</v>
       </c>
-      <c r="H4" s="136">
+      <c r="H4" s="121">
         <f>(C4-C11)/C18</f>
         <v>18.028985507246375</v>
       </c>
-      <c r="I4" s="136">
+      <c r="I4" s="121">
         <f t="shared" ref="I4:J4" si="0">(D4-D11)/D18</f>
         <v>16.982035928143713</v>
       </c>
-      <c r="J4" s="136">
+      <c r="J4" s="121">
         <f t="shared" si="0"/>
         <v>23.166666666666668</v>
       </c>
@@ -4984,15 +4978,15 @@
       <c r="G5" s="15">
         <v>2010</v>
       </c>
-      <c r="H5" s="136">
+      <c r="H5" s="121">
         <f t="shared" ref="H5:I5" si="1">(C5-C12)/C19</f>
         <v>19.044088176352705</v>
       </c>
-      <c r="I5" s="136">
+      <c r="I5" s="121">
         <f t="shared" si="1"/>
         <v>23.985714285714284</v>
       </c>
-      <c r="J5" s="135"/>
+      <c r="J5" s="120"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B6" s="15">
@@ -5006,35 +5000,35 @@
       <c r="G6" s="15">
         <v>2011</v>
       </c>
-      <c r="H6" s="136">
+      <c r="H6" s="121">
         <f>(C6-C13)/C20</f>
         <v>22.519540229885056</v>
       </c>
-      <c r="I6" s="138" t="s">
+      <c r="I6" s="123" t="s">
         <v>357</v>
       </c>
-      <c r="J6" s="135"/>
+      <c r="J6" s="120"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B9" s="121" t="s">
+      <c r="B9" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="119" t="s">
+      <c r="C9" s="156" t="s">
         <v>312</v>
       </c>
-      <c r="D9" s="119"/>
-      <c r="E9" s="119"/>
-      <c r="G9" s="121" t="s">
+      <c r="D9" s="156"/>
+      <c r="E9" s="156"/>
+      <c r="G9" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="H9" s="119" t="s">
+      <c r="H9" s="156" t="s">
         <v>349</v>
       </c>
-      <c r="I9" s="119"/>
-      <c r="J9" s="119"/>
+      <c r="I9" s="156"/>
+      <c r="J9" s="156"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B10" s="121"/>
+      <c r="B10" s="159"/>
       <c r="C10" s="2" t="s">
         <v>4</v>
       </c>
@@ -5044,7 +5038,7 @@
       <c r="E10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="121"/>
+      <c r="G10" s="159"/>
       <c r="H10" s="2" t="s">
         <v>4</v>
       </c>
@@ -5071,15 +5065,15 @@
       <c r="G11" s="15" t="s">
         <v>350</v>
       </c>
-      <c r="H11" s="137">
+      <c r="H11" s="122">
         <f>H5/H4-1</f>
         <v>5.6303926180335084E-2</v>
       </c>
-      <c r="I11" s="137">
+      <c r="I11" s="122">
         <f>I5/I4-1</f>
         <v>0.41241688494861961</v>
       </c>
-      <c r="J11" s="136"/>
+      <c r="J11" s="121"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B12" s="15">
@@ -5095,14 +5089,14 @@
       <c r="G12" s="15" t="s">
         <v>351</v>
       </c>
-      <c r="H12" s="137">
+      <c r="H12" s="122">
         <f>H6/H5-1</f>
         <v>0.18249506205541866</v>
       </c>
-      <c r="I12" s="139" t="s">
+      <c r="I12" s="124" t="s">
         <v>358</v>
       </c>
-      <c r="J12" s="135"/>
+      <c r="J12" s="120"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B13" s="15">
@@ -5114,9 +5108,9 @@
       <c r="D13" s="33"/>
       <c r="E13" s="33"/>
       <c r="G13" s="15"/>
-      <c r="H13" s="136"/>
-      <c r="I13" s="135"/>
-      <c r="J13" s="135"/>
+      <c r="H13" s="121"/>
+      <c r="I13" s="120"/>
+      <c r="J13" s="120"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.2">
       <c r="G14" s="1" t="s">
@@ -5125,25 +5119,25 @@
       <c r="H14" s="1"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B16" s="121" t="s">
+      <c r="B16" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="119" t="s">
+      <c r="C16" s="156" t="s">
         <v>348</v>
       </c>
-      <c r="D16" s="119"/>
-      <c r="E16" s="119"/>
-      <c r="G16" s="121" t="s">
+      <c r="D16" s="156"/>
+      <c r="E16" s="156"/>
+      <c r="G16" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="H16" s="119" t="s">
+      <c r="H16" s="156" t="s">
         <v>353</v>
       </c>
-      <c r="I16" s="119"/>
-      <c r="J16" s="119"/>
+      <c r="I16" s="156"/>
+      <c r="J16" s="156"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B17" s="121"/>
+      <c r="B17" s="159"/>
       <c r="C17" s="2" t="s">
         <v>4</v>
       </c>
@@ -5153,7 +5147,7 @@
       <c r="E17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="121"/>
+      <c r="G17" s="159"/>
       <c r="H17" s="2" t="s">
         <v>4</v>
       </c>
@@ -5180,15 +5174,15 @@
       <c r="G18" s="15">
         <v>2009</v>
       </c>
-      <c r="H18" s="136">
+      <c r="H18" s="121">
         <f>H$6*(1+$C$23)^($G18+(VALUE(LEFT(H$17,2))/12-1)-$G$20)</f>
         <v>19.306876054428201</v>
       </c>
-      <c r="I18" s="136">
+      <c r="I18" s="121">
         <f>I$5*(1+$C$23)^($G18+(VALUE(LEFT(I$17,2))/12-1)-$G$20)</f>
         <v>22.208994708994705</v>
       </c>
-      <c r="J18" s="136">
+      <c r="J18" s="121">
         <f>J$4*(1+$C$23)^($G18+(VALUE(LEFT(J$17,2))/12-1)-$G$20)</f>
         <v>23.166666666666668</v>
       </c>
@@ -5207,15 +5201,15 @@
       <c r="G19" s="15">
         <v>2010</v>
       </c>
-      <c r="H19" s="136">
+      <c r="H19" s="121">
         <f t="shared" ref="H19" si="2">H$6*(1+$C$23)^($G19+(VALUE(LEFT(H$17,2))/12-1)-$G$20)</f>
         <v>20.851426138782458</v>
       </c>
-      <c r="I19" s="136">
+      <c r="I19" s="121">
         <f>I$5*(1+$C$23)^($G19+(VALUE(LEFT(I$17,2))/12-1)-$G$20)</f>
         <v>23.985714285714284</v>
       </c>
-      <c r="J19" s="138" t="s">
+      <c r="J19" s="123" t="s">
         <v>361</v>
       </c>
     </row>
@@ -5231,14 +5225,14 @@
       <c r="G20" s="15">
         <v>2011</v>
       </c>
-      <c r="H20" s="136">
+      <c r="H20" s="121">
         <f>H$6*(1+$C$23)^($G20+(VALUE(LEFT(H$17,2))/12-1)-$G$20)</f>
         <v>22.519540229885056</v>
       </c>
-      <c r="I20" s="138" t="s">
+      <c r="I20" s="123" t="s">
         <v>360</v>
       </c>
-      <c r="J20" s="135"/>
+      <c r="J20" s="120"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H21" s="7" t="s">
@@ -5252,17 +5246,17 @@
       <c r="C23" s="77">
         <v>0.08</v>
       </c>
-      <c r="G23" s="121" t="s">
+      <c r="G23" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="H23" s="119" t="s">
+      <c r="H23" s="156" t="s">
         <v>354</v>
       </c>
-      <c r="I23" s="119"/>
-      <c r="J23" s="119"/>
+      <c r="I23" s="156"/>
+      <c r="J23" s="156"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="G24" s="121"/>
+      <c r="G24" s="159"/>
       <c r="H24" s="2" t="s">
         <v>4</v>
       </c>
@@ -5277,15 +5271,15 @@
       <c r="G25" s="15">
         <v>2009</v>
       </c>
-      <c r="H25" s="135">
+      <c r="H25" s="120">
         <f>H18*C18+C11</f>
         <v>10371.872238777731</v>
       </c>
-      <c r="I25" s="135">
+      <c r="I25" s="120">
         <f t="shared" ref="I25" si="3">I18*D18+D11</f>
         <v>12455.902116402116</v>
       </c>
-      <c r="J25" s="135">
+      <c r="J25" s="120">
         <f>J18*E18+E11</f>
         <v>13053</v>
       </c>
@@ -5294,11 +5288,11 @@
       <c r="G26" s="15">
         <v>2010</v>
       </c>
-      <c r="H26" s="135">
+      <c r="H26" s="120">
         <f t="shared" ref="H26:I26" si="4">H19*C19+C12</f>
         <v>13868.861643252447</v>
       </c>
-      <c r="I26" s="135">
+      <c r="I26" s="120">
         <f t="shared" si="4"/>
         <v>17391</v>
       </c>
@@ -5308,11 +5302,11 @@
       <c r="G27" s="15">
         <v>2011</v>
       </c>
-      <c r="H27" s="135">
+      <c r="H27" s="120">
         <f>H20*C20+C13</f>
         <v>12924</v>
       </c>
-      <c r="I27" s="138" t="s">
+      <c r="I27" s="123" t="s">
         <v>362</v>
       </c>
       <c r="J27" s="33"/>
@@ -5324,17 +5318,17 @@
       <c r="I28" s="1"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="G30" s="121" t="s">
+      <c r="G30" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="H30" s="119" t="s">
+      <c r="H30" s="156" t="s">
         <v>356</v>
       </c>
-      <c r="I30" s="119"/>
-      <c r="J30" s="125"/>
+      <c r="I30" s="156"/>
+      <c r="J30" s="2"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="G31" s="121"/>
+      <c r="G31" s="159"/>
       <c r="H31" s="2" t="s">
         <v>320</v>
       </c>
@@ -5355,7 +5349,7 @@
         <f>J25/I25</f>
         <v>1.0479369441103441</v>
       </c>
-      <c r="J32" s="135"/>
+      <c r="J32" s="120"/>
     </row>
     <row r="33" spans="7:10" x14ac:dyDescent="0.2">
       <c r="G33" s="15">
@@ -5365,7 +5359,7 @@
         <f>I26/H26</f>
         <v>1.2539601625098886</v>
       </c>
-      <c r="I33" s="128" t="s">
+      <c r="I33" s="114" t="s">
         <v>363</v>
       </c>
       <c r="J33" s="33"/>
@@ -5411,6 +5405,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:E16"/>
     <mergeCell ref="G23:G24"/>
     <mergeCell ref="H23:J23"/>
     <mergeCell ref="G30:G31"/>
@@ -5421,12 +5421,6 @@
     <mergeCell ref="H9:J9"/>
     <mergeCell ref="G16:G17"/>
     <mergeCell ref="H16:J16"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:E16"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5516,7 +5510,7 @@
       <c r="D4" s="16">
         <v>345000</v>
       </c>
-      <c r="E4" s="141">
+      <c r="E4" s="126">
         <f>($C$16-B4+1)*12</f>
         <v>36</v>
       </c>
@@ -5555,7 +5549,7 @@
       <c r="D5" s="16">
         <v>300000</v>
       </c>
-      <c r="E5" s="141">
+      <c r="E5" s="126">
         <f t="shared" ref="E5:E6" si="0">($C$16-B5+1)*12</f>
         <v>24</v>
       </c>
@@ -5594,7 +5588,7 @@
       <c r="D6" s="16">
         <v>235000</v>
       </c>
-      <c r="E6" s="141">
+      <c r="E6" s="126">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -5652,7 +5646,7 @@
       <c r="J10" s="12" t="s">
         <v>277</v>
       </c>
-      <c r="K10" s="143">
+      <c r="K10" s="128">
         <f>SUM(K4:K6)</f>
         <v>89875.406684412883</v>
       </c>
@@ -5700,7 +5694,7 @@
       <c r="B16" s="12" t="s">
         <v>371</v>
       </c>
-      <c r="C16" s="134">
+      <c r="C16" s="119">
         <v>2022</v>
       </c>
       <c r="R16" s="7" t="s">
@@ -5728,7 +5722,7 @@
       <c r="B18" s="12" t="s">
         <v>370</v>
       </c>
-      <c r="C18" s="134">
+      <c r="C18" s="119">
         <v>2024</v>
       </c>
       <c r="N18" s="15">
@@ -5789,7 +5783,7 @@
       <c r="O23" s="39" t="s">
         <v>124</v>
       </c>
-      <c r="Q23" s="144" t="s">
+      <c r="Q23" s="129" t="s">
         <v>390</v>
       </c>
       <c r="R23" s="12" t="s">
@@ -5811,7 +5805,7 @@
       <c r="O24" s="15">
         <v>2.5</v>
       </c>
-      <c r="Q24" s="144" t="s">
+      <c r="Q24" s="129" t="s">
         <v>389</v>
       </c>
       <c r="R24" s="12" t="s">
@@ -5836,7 +5830,7 @@
       <c r="O25" s="15">
         <v>2.0499999999999998</v>
       </c>
-      <c r="Q25" s="144" t="s">
+      <c r="Q25" s="129" t="s">
         <v>391</v>
       </c>
       <c r="R25" s="12" t="s">
@@ -5847,7 +5841,7 @@
         <v>48</v>
       </c>
       <c r="T25" s="5">
-        <f t="shared" ref="T24:T25" si="6">_xlfn.XLOOKUP(S25,$N$24:$N$28,$O$24:$O$28)</f>
+        <f t="shared" ref="T25" si="6">_xlfn.XLOOKUP(S25,$N$24:$N$28,$O$24:$O$28)</f>
         <v>1.4</v>
       </c>
     </row>
@@ -5866,7 +5860,7 @@
       <c r="O27" s="15">
         <v>1.4</v>
       </c>
-      <c r="R27" s="146" t="s">
+      <c r="R27" s="131" t="s">
         <v>395</v>
       </c>
     </row>
@@ -5877,7 +5871,7 @@
       <c r="O28" s="15">
         <v>1.1499999999999999</v>
       </c>
-      <c r="R28" s="145" t="str">
+      <c r="R28" s="130" t="str">
         <f>"AY 2021 Exp Paid Claims between "&amp;$S$23&amp;" - "&amp;S24&amp;" months = "</f>
         <v xml:space="preserve">AY 2021 Exp Paid Claims between 24 - 36 months = </v>
       </c>
@@ -5890,7 +5884,7 @@
       </c>
     </row>
     <row r="29" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="R29" s="145" t="str">
+      <c r="R29" s="130" t="str">
         <f>"AY 2021 Exp Paid Claims between "&amp;$S$23&amp;" - "&amp;S25&amp;" months = "</f>
         <v xml:space="preserve">AY 2021 Exp Paid Claims between 24 - 48 months = </v>
       </c>
@@ -5903,7 +5897,7 @@
       <c r="N31" s="12" t="s">
         <v>371</v>
       </c>
-      <c r="O31" s="134">
+      <c r="O31" s="119">
         <v>2022</v>
       </c>
     </row>
@@ -5924,7 +5918,7 @@
       <c r="N34" s="12" t="s">
         <v>381</v>
       </c>
-      <c r="O34" s="142">
+      <c r="O34" s="127">
         <v>45383</v>
       </c>
     </row>
@@ -5951,25 +5945,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B2" s="118" t="s">
+      <c r="B2" s="157" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="119" t="s">
+      <c r="C2" s="156" t="s">
         <v>396</v>
       </c>
-      <c r="D2" s="119"/>
-      <c r="E2" s="119"/>
-      <c r="G2" s="118" t="s">
+      <c r="D2" s="156"/>
+      <c r="E2" s="156"/>
+      <c r="G2" s="157" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="119" t="s">
+      <c r="H2" s="156" t="s">
         <v>402</v>
       </c>
-      <c r="I2" s="119"/>
-      <c r="J2" s="125"/>
+      <c r="I2" s="156"/>
+      <c r="J2" s="2"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B3" s="118"/>
+      <c r="B3" s="157"/>
       <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
@@ -5979,7 +5973,7 @@
       <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="118"/>
+      <c r="G3" s="157"/>
       <c r="H3" s="2" t="s">
         <v>320</v>
       </c>
@@ -6035,7 +6029,7 @@
         <v>1.1172806785051683</v>
       </c>
       <c r="I5" s="8"/>
-      <c r="J5" s="135"/>
+      <c r="J5" s="120"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B6" s="15">
@@ -6071,18 +6065,18 @@
       <c r="G8" s="12"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B9" s="118" t="s">
+      <c r="B9" s="157" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="119" t="s">
+      <c r="C9" s="156" t="s">
         <v>397</v>
       </c>
-      <c r="D9" s="119"/>
-      <c r="E9" s="119"/>
+      <c r="D9" s="156"/>
+      <c r="E9" s="156"/>
       <c r="G9" s="12" t="s">
         <v>403</v>
       </c>
-      <c r="H9" s="147">
+      <c r="H9" s="132">
         <f>PRODUCT(H7:I7)</f>
         <v>1.1193666738427805</v>
       </c>
@@ -6091,7 +6085,7 @@
       </c>
     </row>
     <row r="10" spans="2:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="118"/>
+      <c r="B10" s="157"/>
       <c r="C10" s="2" t="s">
         <v>4</v>
       </c>
@@ -6127,14 +6121,14 @@
         <v>4657</v>
       </c>
       <c r="E12" s="33"/>
-      <c r="G12" s="118" t="s">
+      <c r="G12" s="157" t="s">
         <v>3</v>
       </c>
-      <c r="H12" s="119" t="s">
+      <c r="H12" s="156" t="s">
         <v>400</v>
       </c>
-      <c r="I12" s="119"/>
-      <c r="J12" s="119"/>
+      <c r="I12" s="156"/>
+      <c r="J12" s="156"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B13" s="15">
@@ -6145,7 +6139,7 @@
       </c>
       <c r="D13" s="33"/>
       <c r="E13" s="33"/>
-      <c r="G13" s="118"/>
+      <c r="G13" s="157"/>
       <c r="H13" s="2" t="s">
         <v>4</v>
       </c>
@@ -6188,7 +6182,7 @@
         <f>D12/D5</f>
         <v>0.27618313367334835</v>
       </c>
-      <c r="J15" s="135"/>
+      <c r="J15" s="120"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
@@ -6226,7 +6220,7 @@
       <c r="G18" s="12" t="s">
         <v>405</v>
       </c>
-      <c r="H18" s="147">
+      <c r="H18" s="132">
         <f>H16*C19</f>
         <v>0.28146771236504381</v>
       </c>
@@ -6316,28 +6310,28 @@
       </c>
     </row>
     <row r="3" spans="2:9" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="148" t="s">
+      <c r="B3" s="133" t="s">
         <v>414</v>
       </c>
-      <c r="C3" s="148" t="s">
+      <c r="C3" s="133" t="s">
         <v>415</v>
       </c>
-      <c r="D3" s="148" t="s">
+      <c r="D3" s="133" t="s">
         <v>416</v>
       </c>
-      <c r="E3" s="148" t="s">
+      <c r="E3" s="133" t="s">
         <v>417</v>
       </c>
-      <c r="F3" s="148" t="s">
+      <c r="F3" s="133" t="s">
         <v>418</v>
       </c>
-      <c r="G3" s="148" t="s">
+      <c r="G3" s="133" t="s">
         <v>419</v>
       </c>
-      <c r="H3" s="148" t="s">
+      <c r="H3" s="133" t="s">
         <v>420</v>
       </c>
-      <c r="I3" s="148" t="s">
+      <c r="I3" s="133" t="s">
         <v>421</v>
       </c>
     </row>
@@ -6462,7 +6456,7 @@
       <c r="H10" t="s">
         <v>277</v>
       </c>
-      <c r="I10" s="140">
+      <c r="I10" s="125">
         <f>SUM(I4:I7)*1000</f>
         <v>9869689.9999999981</v>
       </c>
@@ -6557,15 +6551,15 @@
         <f>($B$7-B4+1)*12</f>
         <v>48</v>
       </c>
-      <c r="F4" s="153">
+      <c r="F4" s="137">
         <f>_xlfn.XLOOKUP(E4,$K$9:$M$9,$K$19:$M$19,0)</f>
         <v>0</v>
       </c>
-      <c r="G4" s="153">
+      <c r="G4" s="137">
         <f>MAX(_xlfn.XLOOKUP(B4,$B$13:$B$16,$C$13:$F$16))</f>
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="H4" s="153">
+      <c r="H4" s="137">
         <f>SUM(F4:G4)</f>
         <v>4.8000000000000001E-2</v>
       </c>
@@ -6596,20 +6590,20 @@
         <f t="shared" ref="E5:E7" si="0">($B$7-B5+1)*12</f>
         <v>36</v>
       </c>
-      <c r="F5" s="153">
+      <c r="F5" s="137">
         <f>_xlfn.XLOOKUP(E5,$K$9:$M$9,$K$19:$M$19,0)</f>
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="G5" s="153">
+      <c r="G5" s="137">
         <f t="shared" ref="G5:G7" si="1">MAX(_xlfn.XLOOKUP(B5,$B$13:$B$16,$C$13:$F$16))</f>
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="H5" s="153">
+      <c r="H5" s="137">
         <f t="shared" ref="H5:H7" si="2">SUM(F5:G5)</f>
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="I5" s="29">
-        <f t="shared" ref="I5:I7" si="3">C5*H5</f>
+        <f t="shared" ref="I5:I6" si="3">C5*H5</f>
         <v>2812.5</v>
       </c>
       <c r="J5" s="28">
@@ -6631,15 +6625,15 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="F6" s="153">
+      <c r="F6" s="137">
         <f>_xlfn.XLOOKUP(E6,$K$9:$M$9,$K$19:$M$19,0)</f>
         <v>1.9E-2</v>
       </c>
-      <c r="G6" s="153">
+      <c r="G6" s="137">
         <f t="shared" si="1"/>
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="H6" s="153">
+      <c r="H6" s="137">
         <f t="shared" si="2"/>
         <v>4.4999999999999998E-2</v>
       </c>
@@ -6666,15 +6660,15 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="F7" s="153">
+      <c r="F7" s="137">
         <f>_xlfn.XLOOKUP(E7,$K$9:$M$9,$K$19:$M$19,0)</f>
         <v>2.4666666666666667E-2</v>
       </c>
-      <c r="G7" s="153">
+      <c r="G7" s="137">
         <f t="shared" si="1"/>
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="H7" s="153">
+      <c r="H7" s="137">
         <f t="shared" si="2"/>
         <v>4.6666666666666662E-2</v>
       </c>
@@ -6707,7 +6701,7 @@
         <v>12</v>
       </c>
       <c r="L9" s="5">
-        <f t="shared" ref="L9:M9" si="4">VALUE(LEFT(L12,2))</f>
+        <f t="shared" ref="L9" si="4">VALUE(LEFT(L12,2))</f>
         <v>24</v>
       </c>
       <c r="M9" s="5">
@@ -6716,47 +6710,47 @@
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B10" s="119" t="s">
+      <c r="B10" s="156" t="s">
         <v>426</v>
       </c>
-      <c r="C10" s="119"/>
-      <c r="D10" s="119"/>
-      <c r="E10" s="119"/>
-      <c r="F10" s="119"/>
+      <c r="C10" s="156"/>
+      <c r="D10" s="156"/>
+      <c r="E10" s="156"/>
+      <c r="F10" s="156"/>
       <c r="G10" s="47"/>
       <c r="H10" s="47"/>
-      <c r="J10" s="119" t="s">
+      <c r="J10" s="156" t="s">
         <v>427</v>
       </c>
-      <c r="K10" s="119"/>
-      <c r="L10" s="119"/>
-      <c r="M10" s="119"/>
-      <c r="N10" s="125"/>
+      <c r="K10" s="156"/>
+      <c r="L10" s="156"/>
+      <c r="M10" s="156"/>
+      <c r="N10" s="2"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B11" s="149" t="s">
+      <c r="B11" s="162" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="119" t="s">
+      <c r="C11" s="156" t="s">
         <v>262</v>
       </c>
-      <c r="D11" s="119"/>
-      <c r="E11" s="119"/>
-      <c r="F11" s="119"/>
+      <c r="D11" s="156"/>
+      <c r="E11" s="156"/>
+      <c r="F11" s="156"/>
       <c r="G11" s="47"/>
       <c r="H11" s="47"/>
-      <c r="J11" s="118" t="s">
+      <c r="J11" s="157" t="s">
         <v>3</v>
       </c>
-      <c r="K11" s="119" t="s">
+      <c r="K11" s="156" t="s">
         <v>428</v>
       </c>
-      <c r="L11" s="119"/>
-      <c r="M11" s="119"/>
-      <c r="N11" s="125"/>
+      <c r="L11" s="156"/>
+      <c r="M11" s="156"/>
+      <c r="N11" s="2"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B12" s="149"/>
+      <c r="B12" s="162"/>
       <c r="C12" s="2">
         <v>12</v>
       </c>
@@ -6771,7 +6765,7 @@
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-      <c r="J12" s="118"/>
+      <c r="J12" s="157"/>
       <c r="K12" s="79" t="s">
         <v>9</v>
       </c>
@@ -6787,36 +6781,36 @@
       <c r="B13" s="15">
         <v>2003</v>
       </c>
-      <c r="C13" s="150">
+      <c r="C13" s="134">
         <v>2.4E-2</v>
       </c>
-      <c r="D13" s="150">
+      <c r="D13" s="134">
         <v>0.03</v>
       </c>
-      <c r="E13" s="150">
+      <c r="E13" s="134">
         <v>0.04</v>
       </c>
-      <c r="F13" s="150">
+      <c r="F13" s="134">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="G13" s="150"/>
-      <c r="H13" s="150"/>
+      <c r="G13" s="134"/>
+      <c r="H13" s="134"/>
       <c r="J13" s="15">
         <v>2003</v>
       </c>
-      <c r="K13" s="151">
+      <c r="K13" s="135">
         <f>D13-C13</f>
         <v>5.9999999999999984E-3</v>
       </c>
-      <c r="L13" s="151">
+      <c r="L13" s="135">
         <f>E13-D13</f>
         <v>1.0000000000000002E-2</v>
       </c>
-      <c r="M13" s="151">
+      <c r="M13" s="135">
         <f>F13-E13</f>
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="N13" s="154" t="s">
+      <c r="N13" s="138" t="s">
         <v>433</v>
       </c>
     </row>
@@ -6824,88 +6818,88 @@
       <c r="B14" s="15">
         <v>2004</v>
       </c>
-      <c r="C14" s="150">
+      <c r="C14" s="134">
         <v>0.02</v>
       </c>
-      <c r="D14" s="150">
+      <c r="D14" s="134">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="E14" s="150">
+      <c r="E14" s="134">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="F14" s="150"/>
-      <c r="G14" s="150"/>
-      <c r="H14" s="150"/>
+      <c r="F14" s="134"/>
+      <c r="G14" s="134"/>
+      <c r="H14" s="134"/>
       <c r="J14" s="15">
         <v>2004</v>
       </c>
-      <c r="K14" s="151">
+      <c r="K14" s="135">
         <f t="shared" ref="K14:K15" si="5">D14-C14</f>
         <v>5.000000000000001E-3</v>
       </c>
-      <c r="L14" s="151">
+      <c r="L14" s="135">
         <f>E14-D14</f>
         <v>1.1999999999999997E-2</v>
       </c>
-      <c r="M14" s="151"/>
-      <c r="N14" s="150"/>
+      <c r="M14" s="135"/>
+      <c r="N14" s="134"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B15" s="15">
         <v>2005</v>
       </c>
-      <c r="C15" s="150">
+      <c r="C15" s="134">
         <v>0.02</v>
       </c>
-      <c r="D15" s="150">
+      <c r="D15" s="134">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="E15" s="150"/>
-      <c r="F15" s="150"/>
-      <c r="G15" s="150"/>
-      <c r="H15" s="150"/>
+      <c r="E15" s="134"/>
+      <c r="F15" s="134"/>
+      <c r="G15" s="134"/>
+      <c r="H15" s="134"/>
       <c r="J15" s="15">
         <v>2005</v>
       </c>
-      <c r="K15" s="151">
+      <c r="K15" s="135">
         <f t="shared" si="5"/>
         <v>5.9999999999999984E-3</v>
       </c>
-      <c r="L15" s="151"/>
-      <c r="M15" s="151"/>
-      <c r="N15" s="150"/>
+      <c r="L15" s="135"/>
+      <c r="M15" s="135"/>
+      <c r="N15" s="134"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B16" s="15">
         <v>2006</v>
       </c>
-      <c r="C16" s="150">
+      <c r="C16" s="134">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="D16" s="150"/>
-      <c r="E16" s="150"/>
-      <c r="F16" s="150"/>
-      <c r="G16" s="150"/>
-      <c r="H16" s="150"/>
+      <c r="D16" s="134"/>
+      <c r="E16" s="134"/>
+      <c r="F16" s="134"/>
+      <c r="G16" s="134"/>
+      <c r="H16" s="134"/>
       <c r="J16" s="15"/>
-      <c r="K16" s="150"/>
-      <c r="L16" s="150"/>
-      <c r="M16" s="150"/>
-      <c r="N16" s="150"/>
+      <c r="K16" s="134"/>
+      <c r="L16" s="134"/>
+      <c r="M16" s="134"/>
+      <c r="N16" s="134"/>
     </row>
     <row r="17" spans="10:14" x14ac:dyDescent="0.2">
       <c r="J17" t="s">
         <v>401</v>
       </c>
-      <c r="K17" s="152">
+      <c r="K17" s="136">
         <f>AVERAGE(K13:K15)</f>
         <v>5.6666666666666662E-3</v>
       </c>
-      <c r="L17" s="152">
+      <c r="L17" s="136">
         <f t="shared" ref="L17" si="6">AVERAGE(L13:L15)</f>
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="M17" s="152">
+      <c r="M17" s="136">
         <f>AVERAGE(M13:M15)</f>
         <v>8.0000000000000002E-3</v>
       </c>
@@ -6917,15 +6911,15 @@
       <c r="J19" t="s">
         <v>21</v>
       </c>
-      <c r="K19" s="152">
+      <c r="K19" s="136">
         <f>SUM(K17:$M$17)</f>
         <v>2.4666666666666667E-2</v>
       </c>
-      <c r="L19" s="152">
+      <c r="L19" s="136">
         <f>SUM(L17:$M$17)</f>
         <v>1.9E-2</v>
       </c>
-      <c r="M19" s="152">
+      <c r="M19" s="136">
         <f>SUM(M17:$M$17)</f>
         <v>8.0000000000000002E-3</v>
       </c>
@@ -6968,46 +6962,46 @@
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B2" s="2"/>
-      <c r="C2" s="149" t="s">
+      <c r="C2" s="162" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="149"/>
-      <c r="E2" s="149"/>
-      <c r="F2" s="149"/>
-      <c r="G2" s="149"/>
+      <c r="D2" s="162"/>
+      <c r="E2" s="162"/>
+      <c r="F2" s="162"/>
+      <c r="G2" s="162"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="149" t="s">
+      <c r="J2" s="162" t="s">
         <v>63</v>
       </c>
-      <c r="K2" s="149"/>
-      <c r="L2" s="149"/>
-      <c r="M2" s="149"/>
-      <c r="N2" s="149"/>
+      <c r="K2" s="162"/>
+      <c r="L2" s="162"/>
+      <c r="M2" s="162"/>
+      <c r="N2" s="162"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B3" s="149" t="s">
+      <c r="B3" s="162" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="119" t="s">
+      <c r="C3" s="156" t="s">
         <v>445</v>
       </c>
-      <c r="D3" s="119"/>
-      <c r="E3" s="119"/>
-      <c r="F3" s="119"/>
-      <c r="G3" s="119"/>
-      <c r="I3" s="149" t="s">
+      <c r="D3" s="156"/>
+      <c r="E3" s="156"/>
+      <c r="F3" s="156"/>
+      <c r="G3" s="156"/>
+      <c r="I3" s="162" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="119" t="s">
+      <c r="J3" s="156" t="s">
         <v>445</v>
       </c>
-      <c r="K3" s="119"/>
-      <c r="L3" s="119"/>
-      <c r="M3" s="119"/>
-      <c r="N3" s="119"/>
+      <c r="K3" s="156"/>
+      <c r="L3" s="156"/>
+      <c r="M3" s="156"/>
+      <c r="N3" s="156"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B4" s="149"/>
+      <c r="B4" s="162"/>
       <c r="C4" s="2">
         <v>12</v>
       </c>
@@ -7023,7 +7017,7 @@
       <c r="G4" s="2">
         <v>60</v>
       </c>
-      <c r="I4" s="149"/>
+      <c r="I4" s="162"/>
       <c r="J4" s="2">
         <v>12</v>
       </c>
@@ -7065,19 +7059,19 @@
       <c r="J5" s="33">
         <v>10000</v>
       </c>
-      <c r="K5" s="135">
+      <c r="K5" s="120">
         <f>D5-C5</f>
         <v>2500</v>
       </c>
-      <c r="L5" s="135">
+      <c r="L5" s="120">
         <f t="shared" ref="L5:N6" si="0">E5-D5</f>
         <v>3000</v>
       </c>
-      <c r="M5" s="135">
+      <c r="M5" s="120">
         <f t="shared" si="0"/>
         <v>1500</v>
       </c>
-      <c r="N5" s="135">
+      <c r="N5" s="120">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
@@ -7105,19 +7099,19 @@
       <c r="J6" s="33">
         <v>11000</v>
       </c>
-      <c r="K6" s="135">
-        <f t="shared" ref="K6:L8" si="1">D6-C6</f>
+      <c r="K6" s="120">
+        <f t="shared" ref="K6:L7" si="1">D6-C6</f>
         <v>2000</v>
       </c>
-      <c r="L6" s="135">
+      <c r="L6" s="120">
         <f t="shared" si="0"/>
         <v>3000</v>
       </c>
-      <c r="M6" s="135">
+      <c r="M6" s="120">
         <f t="shared" si="0"/>
         <v>2000</v>
       </c>
-      <c r="N6" s="135"/>
+      <c r="N6" s="120"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B7" s="15">
@@ -7140,16 +7134,16 @@
       <c r="J7" s="33">
         <v>9500</v>
       </c>
-      <c r="K7" s="135">
+      <c r="K7" s="120">
         <f t="shared" si="1"/>
         <v>2500</v>
       </c>
-      <c r="L7" s="135">
+      <c r="L7" s="120">
         <f t="shared" si="1"/>
         <v>3000</v>
       </c>
-      <c r="M7" s="135"/>
-      <c r="N7" s="135"/>
+      <c r="M7" s="120"/>
+      <c r="N7" s="120"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B8" s="15">
@@ -7170,15 +7164,15 @@
       <c r="J8" s="33">
         <v>10200</v>
       </c>
-      <c r="K8" s="135">
+      <c r="K8" s="120">
         <f>D8-C8</f>
         <v>2800</v>
       </c>
-      <c r="L8" s="138" t="s">
+      <c r="L8" s="123" t="s">
         <v>461</v>
       </c>
-      <c r="M8" s="135"/>
-      <c r="N8" s="135"/>
+      <c r="M8" s="120"/>
+      <c r="N8" s="120"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B9" s="15">
@@ -7197,10 +7191,10 @@
       <c r="J9" s="33">
         <v>11200</v>
       </c>
-      <c r="K9" s="135"/>
-      <c r="L9" s="135"/>
-      <c r="M9" s="135"/>
-      <c r="N9" s="135"/>
+      <c r="K9" s="120"/>
+      <c r="L9" s="120"/>
+      <c r="M9" s="120"/>
+      <c r="N9" s="120"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.2">
       <c r="E11" s="7" t="s">
@@ -7286,34 +7280,34 @@
       </c>
     </row>
     <row r="17" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="155">
+      <c r="B17" s="139">
         <v>2003</v>
       </c>
-      <c r="C17" s="156">
+      <c r="C17" s="140">
         <v>2800</v>
       </c>
-      <c r="D17" s="157">
+      <c r="D17" s="141">
         <f>SUM(J9,K8,L7,M6,N5)</f>
         <v>20000</v>
       </c>
-      <c r="E17" s="158">
+      <c r="E17" s="142">
         <f t="shared" si="2"/>
         <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="18" spans="2:22" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="159"/>
-      <c r="C18" s="160"/>
-      <c r="D18" s="163" t="s">
+      <c r="B18" s="15"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="143" t="s">
         <v>457</v>
       </c>
-      <c r="E18" s="162"/>
+      <c r="E18" s="9"/>
     </row>
     <row r="19" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B19" s="159"/>
-      <c r="C19" s="160"/>
-      <c r="D19" s="161"/>
-      <c r="E19" s="162"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="9"/>
     </row>
     <row r="20" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D20" t="s">
@@ -7457,7 +7451,7 @@
       <c r="P33" s="40" t="s">
         <v>450</v>
       </c>
-      <c r="Q33" s="164">
+      <c r="Q33" s="144">
         <v>0.5</v>
       </c>
     </row>
@@ -7466,7 +7460,7 @@
       <c r="P34" s="40" t="s">
         <v>451</v>
       </c>
-      <c r="Q34" s="164">
+      <c r="Q34" s="144">
         <v>0</v>
       </c>
       <c r="T34" s="12" t="s">
@@ -7485,7 +7479,7 @@
       <c r="P35" s="40" t="s">
         <v>452</v>
       </c>
-      <c r="Q35" s="164">
+      <c r="Q35" s="144">
         <v>0.5</v>
       </c>
     </row>
@@ -7599,23 +7593,23 @@
       </c>
     </row>
     <row r="46" spans="15:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="Y46" s="155">
+      <c r="Y46" s="139">
         <v>2010</v>
       </c>
-      <c r="Z46" s="166">
+      <c r="Z46" s="146">
         <v>5500</v>
       </c>
-      <c r="AA46" s="166">
+      <c r="AA46" s="146">
         <v>40000</v>
       </c>
-      <c r="AB46" s="166">
+      <c r="AB46" s="146">
         <v>30100</v>
       </c>
-      <c r="AC46" s="167">
+      <c r="AC46" s="147">
         <f t="shared" si="3"/>
         <v>36040</v>
       </c>
-      <c r="AD46" s="158">
+      <c r="AD46" s="142">
         <f>Z46/AC46</f>
         <v>0.15260821309655939</v>
       </c>
@@ -7637,7 +7631,7 @@
       <c r="Z49" s="40" t="s">
         <v>450</v>
       </c>
-      <c r="AA49" s="164">
+      <c r="AA49" s="144">
         <v>0.6</v>
       </c>
     </row>
@@ -7645,7 +7639,7 @@
       <c r="Z50" s="40" t="s">
         <v>451</v>
       </c>
-      <c r="AA50" s="164">
+      <c r="AA50" s="144">
         <v>0.4</v>
       </c>
       <c r="AD50" s="19" t="s">
@@ -7656,13 +7650,13 @@
       <c r="Z51" s="40" t="s">
         <v>452</v>
       </c>
-      <c r="AA51" s="164">
+      <c r="AA51" s="144">
         <v>0</v>
       </c>
       <c r="AC51" s="12" t="s">
         <v>481</v>
       </c>
-      <c r="AD51" s="168">
+      <c r="AD51" s="148">
         <f>AD48*AA53-SUM(Z43:Z46)</f>
         <v>2999.4435390534782</v>
       </c>
@@ -7674,7 +7668,7 @@
       <c r="Z53" s="40" t="s">
         <v>477</v>
       </c>
-      <c r="AA53" s="165">
+      <c r="AA53" s="145">
         <v>117500</v>
       </c>
     </row>
@@ -7883,27 +7877,27 @@
       <c r="D13" s="16"/>
     </row>
     <row r="15" spans="2:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="117" t="s">
+      <c r="B15" s="155" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="116" t="s">
+      <c r="C15" s="154" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="116"/>
-      <c r="E15" s="116"/>
-      <c r="F15" s="116"/>
-      <c r="H15" s="117" t="s">
+      <c r="D15" s="154"/>
+      <c r="E15" s="154"/>
+      <c r="F15" s="154"/>
+      <c r="H15" s="155" t="s">
         <v>3</v>
       </c>
-      <c r="I15" s="116" t="s">
+      <c r="I15" s="154" t="s">
         <v>69</v>
       </c>
-      <c r="J15" s="116"/>
-      <c r="K15" s="116"/>
-      <c r="L15" s="116"/>
+      <c r="J15" s="154"/>
+      <c r="K15" s="154"/>
+      <c r="L15" s="154"/>
     </row>
     <row r="16" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="117"/>
+      <c r="B16" s="155"/>
       <c r="C16" s="39" t="s">
         <v>4</v>
       </c>
@@ -7916,7 +7910,7 @@
       <c r="F16" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="H16" s="117"/>
+      <c r="H16" s="155"/>
       <c r="I16" s="72" t="s">
         <v>9</v>
       </c>
@@ -8155,19 +8149,19 @@
       </c>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="O32" s="115" t="s">
+      <c r="O32" s="153" t="s">
         <v>3</v>
       </c>
-      <c r="P32" s="116" t="s">
+      <c r="P32" s="154" t="s">
         <v>84</v>
       </c>
-      <c r="Q32" s="116"/>
-      <c r="R32" s="116"/>
-      <c r="S32" s="116"/>
-      <c r="T32" s="116"/>
+      <c r="Q32" s="154"/>
+      <c r="R32" s="154"/>
+      <c r="S32" s="154"/>
+      <c r="T32" s="154"/>
     </row>
     <row r="33" spans="15:20" x14ac:dyDescent="0.2">
-      <c r="O33" s="115"/>
+      <c r="O33" s="153"/>
       <c r="P33" s="39" t="s">
         <v>4</v>
       </c>
@@ -8264,19 +8258,19 @@
       <c r="S38" s="15"/>
     </row>
     <row r="40" spans="15:20" x14ac:dyDescent="0.2">
-      <c r="O40" s="115" t="s">
+      <c r="O40" s="153" t="s">
         <v>3</v>
       </c>
-      <c r="P40" s="116" t="s">
+      <c r="P40" s="154" t="s">
         <v>69</v>
       </c>
-      <c r="Q40" s="116"/>
-      <c r="R40" s="116"/>
-      <c r="S40" s="116"/>
-      <c r="T40" s="116"/>
+      <c r="Q40" s="154"/>
+      <c r="R40" s="154"/>
+      <c r="S40" s="154"/>
+      <c r="T40" s="154"/>
     </row>
     <row r="41" spans="15:20" x14ac:dyDescent="0.2">
-      <c r="O41" s="115"/>
+      <c r="O41" s="153"/>
       <c r="P41" s="72" t="s">
         <v>9</v>
       </c>
@@ -8566,25 +8560,25 @@
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B5" s="118" t="s">
+      <c r="B5" s="157" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="118" t="s">
+      <c r="C5" s="157" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="119" t="s">
+      <c r="D5" s="156" t="s">
         <v>93</v>
       </c>
-      <c r="E5" s="119"/>
-      <c r="F5" s="119"/>
-      <c r="G5" s="119"/>
+      <c r="E5" s="156"/>
+      <c r="F5" s="156"/>
+      <c r="G5" s="156"/>
       <c r="J5" s="7" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B6" s="118"/>
-      <c r="C6" s="118"/>
+      <c r="B6" s="157"/>
+      <c r="C6" s="157"/>
       <c r="D6" s="2">
         <v>12</v>
       </c>
@@ -8778,22 +8772,22 @@
       </c>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="O14" s="118" t="s">
+      <c r="O14" s="157" t="s">
         <v>28</v>
       </c>
-      <c r="P14" s="118" t="s">
+      <c r="P14" s="157" t="s">
         <v>27</v>
       </c>
-      <c r="Q14" s="119" t="s">
+      <c r="Q14" s="156" t="s">
         <v>93</v>
       </c>
-      <c r="R14" s="119"/>
-      <c r="S14" s="119"/>
-      <c r="T14" s="119"/>
+      <c r="R14" s="156"/>
+      <c r="S14" s="156"/>
+      <c r="T14" s="156"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="O15" s="118"/>
-      <c r="P15" s="118"/>
+      <c r="O15" s="157"/>
+      <c r="P15" s="157"/>
       <c r="Q15" s="2">
         <v>12</v>
       </c>
@@ -9729,18 +9723,18 @@
       <c r="AB22" s="19"/>
     </row>
     <row r="23" spans="2:28" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="M23" s="120" t="s">
+      <c r="M23" s="158" t="s">
         <v>3</v>
       </c>
-      <c r="N23" s="120" t="s">
+      <c r="N23" s="158" t="s">
         <v>27</v>
       </c>
-      <c r="O23" s="116" t="s">
+      <c r="O23" s="154" t="s">
         <v>165</v>
       </c>
-      <c r="P23" s="116"/>
-      <c r="Q23" s="116"/>
-      <c r="R23" s="116"/>
+      <c r="P23" s="154"/>
+      <c r="Q23" s="154"/>
+      <c r="R23" s="154"/>
       <c r="X23" s="19"/>
       <c r="Y23" s="7" t="s">
         <v>180</v>
@@ -9750,14 +9744,14 @@
       <c r="AB23" s="19"/>
     </row>
     <row r="24" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="M24" s="120"/>
-      <c r="N24" s="120"/>
-      <c r="O24" s="116" t="s">
+      <c r="M24" s="158"/>
+      <c r="N24" s="158"/>
+      <c r="O24" s="154" t="s">
         <v>166</v>
       </c>
-      <c r="P24" s="116"/>
-      <c r="Q24" s="116"/>
-      <c r="R24" s="116"/>
+      <c r="P24" s="154"/>
+      <c r="Q24" s="154"/>
+      <c r="R24" s="154"/>
       <c r="T24" s="87"/>
       <c r="U24" s="7" t="s">
         <v>177</v>
@@ -9775,8 +9769,8 @@
       <c r="AB24" s="19"/>
     </row>
     <row r="25" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="M25" s="120"/>
-      <c r="N25" s="120"/>
+      <c r="M25" s="158"/>
+      <c r="N25" s="158"/>
       <c r="O25" s="39">
         <v>12</v>
       </c>
@@ -10029,24 +10023,24 @@
       </c>
     </row>
     <row r="33" spans="13:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="N33" s="116"/>
-      <c r="O33" s="116"/>
-      <c r="P33" s="116"/>
-      <c r="Q33" s="116"/>
+      <c r="N33" s="154"/>
+      <c r="O33" s="154"/>
+      <c r="P33" s="154"/>
+      <c r="Q33" s="154"/>
     </row>
     <row r="34" spans="13:23" x14ac:dyDescent="0.2">
-      <c r="N34" s="120" t="s">
+      <c r="N34" s="158" t="s">
         <v>3</v>
       </c>
-      <c r="O34" s="116" t="s">
+      <c r="O34" s="154" t="s">
         <v>167</v>
       </c>
-      <c r="P34" s="116"/>
-      <c r="Q34" s="116"/>
-      <c r="R34" s="116"/>
+      <c r="P34" s="154"/>
+      <c r="Q34" s="154"/>
+      <c r="R34" s="154"/>
     </row>
     <row r="35" spans="13:23" x14ac:dyDescent="0.2">
-      <c r="N35" s="120"/>
+      <c r="N35" s="158"/>
       <c r="O35" s="72" t="s">
         <v>9</v>
       </c>
@@ -10372,8 +10366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F31610A-B01B-3645-9EE3-5A370BF8379C}">
   <dimension ref="B2:AC42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AH53" sqref="AH53"/>
+    <sheetView topLeftCell="Q14" workbookViewId="0">
+      <selection activeCell="Y18" sqref="Y18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10768,7 +10762,7 @@
         <v>1</v>
       </c>
       <c r="AC32" s="29">
-        <f t="shared" ref="AC32:AC37" si="2">X32*$AA$40*(1-AB32)</f>
+        <f>X32*$AA$40*(1-AB32)</f>
         <v>0</v>
       </c>
     </row>
@@ -10789,15 +10783,15 @@
         <v>1.0529999999999999</v>
       </c>
       <c r="AA33" s="28">
-        <f t="shared" ref="AA33:AA37" si="3">Y33*Z33</f>
+        <f t="shared" ref="AA33:AA37" si="2">Y33*Z33</f>
         <v>3580.2</v>
       </c>
       <c r="AB33" s="96">
-        <f t="shared" ref="AB33:AB37" si="4">1/Z33</f>
+        <f t="shared" ref="AB33:AB37" si="3">1/Z33</f>
         <v>0.94966761633428309</v>
       </c>
       <c r="AC33" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="AC32:AC37" si="4">X33*$AA$40*(1-AB33)</f>
         <v>181.88516426949184</v>
       </c>
     </row>
@@ -10818,15 +10812,15 @@
         <v>1.1759999999999999</v>
       </c>
       <c r="AA34" s="28">
+        <f t="shared" si="2"/>
+        <v>4116</v>
+      </c>
+      <c r="AB34" s="96">
         <f t="shared" si="3"/>
-        <v>4116</v>
-      </c>
-      <c r="AB34" s="96">
+        <v>0.85034013605442182</v>
+      </c>
+      <c r="AC34" s="29">
         <f t="shared" si="4"/>
-        <v>0.85034013605442182</v>
-      </c>
-      <c r="AC34" s="29">
-        <f t="shared" si="2"/>
         <v>624.02649735894295</v>
       </c>
     </row>
@@ -10847,15 +10841,15 @@
         <v>1.429</v>
       </c>
       <c r="AA35" s="28">
+        <f t="shared" si="2"/>
+        <v>4001.2000000000003</v>
+      </c>
+      <c r="AB35" s="96">
         <f t="shared" si="3"/>
-        <v>4001.2000000000003</v>
-      </c>
-      <c r="AB35" s="96">
+        <v>0.69979006298110569</v>
+      </c>
+      <c r="AC35" s="29">
         <f t="shared" si="4"/>
-        <v>0.69979006298110569</v>
-      </c>
-      <c r="AC35" s="29">
-        <f t="shared" si="2"/>
         <v>1301.8354323768979</v>
       </c>
     </row>
@@ -10876,15 +10870,15 @@
         <v>2</v>
       </c>
       <c r="AA36" s="28">
+        <f t="shared" si="2"/>
+        <v>4200</v>
+      </c>
+      <c r="AB36" s="96">
         <f t="shared" si="3"/>
-        <v>4200</v>
-      </c>
-      <c r="AB36" s="96">
+        <v>0.5</v>
+      </c>
+      <c r="AC36" s="25">
         <f t="shared" si="4"/>
-        <v>0.5</v>
-      </c>
-      <c r="AC36" s="25">
-        <f t="shared" si="2"/>
         <v>2168.2084299144371</v>
       </c>
     </row>
@@ -10905,15 +10899,15 @@
         <v>4</v>
       </c>
       <c r="AA37" s="30">
+        <f t="shared" si="2"/>
+        <v>6400</v>
+      </c>
+      <c r="AB37" s="97">
         <f t="shared" si="3"/>
-        <v>6400</v>
-      </c>
-      <c r="AB37" s="97">
+        <v>0.25</v>
+      </c>
+      <c r="AC37" s="31">
         <f t="shared" si="4"/>
-        <v>0.25</v>
-      </c>
-      <c r="AC37" s="31">
-        <f t="shared" si="2"/>
         <v>2918.7421171925112</v>
       </c>
     </row>
@@ -10983,34 +10977,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B2" s="118" t="s">
+      <c r="B2" s="157" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="119" t="s">
+      <c r="C2" s="156" t="s">
         <v>220</v>
       </c>
-      <c r="D2" s="119"/>
-      <c r="E2" s="119"/>
+      <c r="D2" s="156"/>
+      <c r="E2" s="156"/>
       <c r="F2" s="47"/>
-      <c r="G2" s="118" t="s">
+      <c r="G2" s="157" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="119" t="s">
+      <c r="H2" s="156" t="s">
         <v>84</v>
       </c>
-      <c r="I2" s="119"/>
-      <c r="J2" s="119"/>
-      <c r="L2" s="118" t="s">
+      <c r="I2" s="156"/>
+      <c r="J2" s="156"/>
+      <c r="L2" s="157" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="119" t="s">
+      <c r="M2" s="156" t="s">
         <v>226</v>
       </c>
-      <c r="N2" s="119"/>
-      <c r="O2" s="119"/>
+      <c r="N2" s="156"/>
+      <c r="O2" s="156"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B3" s="118"/>
+      <c r="B3" s="157"/>
       <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
@@ -11021,7 +11015,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="2"/>
-      <c r="G3" s="118"/>
+      <c r="G3" s="157"/>
       <c r="H3" s="2" t="s">
         <v>4</v>
       </c>
@@ -11031,7 +11025,7 @@
       <c r="J3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="118"/>
+      <c r="L3" s="157"/>
       <c r="M3" s="2" t="s">
         <v>4</v>
       </c>
@@ -11153,29 +11147,29 @@
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B9" s="118" t="s">
+      <c r="B9" s="157" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="119" t="s">
+      <c r="C9" s="156" t="s">
         <v>221</v>
       </c>
-      <c r="D9" s="119"/>
+      <c r="D9" s="156"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-      <c r="L9" s="118" t="s">
+      <c r="L9" s="157" t="s">
         <v>3</v>
       </c>
-      <c r="M9" s="119" t="s">
+      <c r="M9" s="156" t="s">
         <v>224</v>
       </c>
-      <c r="N9" s="119"/>
+      <c r="N9" s="156"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B10" s="118"/>
+      <c r="B10" s="157"/>
       <c r="C10" s="79" t="s">
         <v>9</v>
       </c>
@@ -11190,7 +11184,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
-      <c r="L10" s="118"/>
+      <c r="L10" s="157"/>
       <c r="M10" s="79" t="s">
         <v>9</v>
       </c>
@@ -11851,59 +11845,59 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B2" s="119" t="s">
+      <c r="B2" s="156" t="s">
         <v>263</v>
       </c>
-      <c r="C2" s="119"/>
-      <c r="D2" s="119"/>
-      <c r="E2" s="119"/>
-      <c r="F2" s="119"/>
-      <c r="I2" s="119" t="s">
+      <c r="C2" s="156"/>
+      <c r="D2" s="156"/>
+      <c r="E2" s="156"/>
+      <c r="F2" s="156"/>
+      <c r="I2" s="156" t="s">
         <v>268</v>
       </c>
-      <c r="J2" s="119"/>
-      <c r="K2" s="119"/>
-      <c r="L2" s="119"/>
-      <c r="M2" s="119"/>
-      <c r="P2" s="119" t="s">
+      <c r="J2" s="156"/>
+      <c r="K2" s="156"/>
+      <c r="L2" s="156"/>
+      <c r="M2" s="156"/>
+      <c r="P2" s="156" t="s">
         <v>272</v>
       </c>
-      <c r="Q2" s="119"/>
-      <c r="R2" s="119"/>
-      <c r="S2" s="119"/>
-      <c r="T2" s="119"/>
+      <c r="Q2" s="156"/>
+      <c r="R2" s="156"/>
+      <c r="S2" s="156"/>
+      <c r="T2" s="156"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B3" s="121" t="s">
+      <c r="B3" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="119" t="s">
+      <c r="C3" s="156" t="s">
         <v>262</v>
       </c>
-      <c r="D3" s="119"/>
-      <c r="E3" s="119"/>
-      <c r="F3" s="119"/>
-      <c r="I3" s="121" t="s">
+      <c r="D3" s="156"/>
+      <c r="E3" s="156"/>
+      <c r="F3" s="156"/>
+      <c r="I3" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="119" t="s">
+      <c r="J3" s="156" t="s">
         <v>262</v>
       </c>
-      <c r="K3" s="119"/>
-      <c r="L3" s="119"/>
-      <c r="M3" s="119"/>
-      <c r="P3" s="121" t="s">
+      <c r="K3" s="156"/>
+      <c r="L3" s="156"/>
+      <c r="M3" s="156"/>
+      <c r="P3" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="Q3" s="119" t="s">
+      <c r="Q3" s="156" t="s">
         <v>262</v>
       </c>
-      <c r="R3" s="119"/>
-      <c r="S3" s="119"/>
-      <c r="T3" s="119"/>
+      <c r="R3" s="156"/>
+      <c r="S3" s="156"/>
+      <c r="T3" s="156"/>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B4" s="121"/>
+      <c r="B4" s="159"/>
       <c r="C4" s="2">
         <v>12</v>
       </c>
@@ -11916,7 +11910,7 @@
       <c r="F4" s="2">
         <v>48</v>
       </c>
-      <c r="I4" s="121"/>
+      <c r="I4" s="159"/>
       <c r="J4" s="2">
         <v>12</v>
       </c>
@@ -11929,7 +11923,7 @@
       <c r="M4" s="2">
         <v>48</v>
       </c>
-      <c r="P4" s="121"/>
+      <c r="P4" s="159"/>
       <c r="Q4" s="2">
         <v>12</v>
       </c>
@@ -12118,22 +12112,22 @@
       <c r="F10" s="15"/>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B11" s="119" t="s">
+      <c r="B11" s="156" t="s">
         <v>265</v>
       </c>
-      <c r="C11" s="119"/>
-      <c r="D11" s="119"/>
-      <c r="E11" s="119"/>
-      <c r="F11" s="119"/>
-      <c r="G11" s="119"/>
-      <c r="I11" s="119" t="s">
+      <c r="C11" s="156"/>
+      <c r="D11" s="156"/>
+      <c r="E11" s="156"/>
+      <c r="F11" s="156"/>
+      <c r="G11" s="156"/>
+      <c r="I11" s="156" t="s">
         <v>267</v>
       </c>
-      <c r="J11" s="119"/>
-      <c r="K11" s="119"/>
-      <c r="L11" s="119"/>
-      <c r="M11" s="119"/>
-      <c r="N11" s="119"/>
+      <c r="J11" s="156"/>
+      <c r="K11" s="156"/>
+      <c r="L11" s="156"/>
+      <c r="M11" s="156"/>
+      <c r="N11" s="156"/>
       <c r="O11" s="47"/>
       <c r="P11" s="3" t="s">
         <v>70</v>
@@ -12156,28 +12150,28 @@
       </c>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B12" s="121" t="s">
+      <c r="B12" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="119" t="s">
+      <c r="C12" s="156" t="s">
         <v>262</v>
       </c>
-      <c r="D12" s="119"/>
-      <c r="E12" s="119"/>
-      <c r="F12" s="119"/>
-      <c r="G12" s="121" t="s">
+      <c r="D12" s="156"/>
+      <c r="E12" s="156"/>
+      <c r="F12" s="156"/>
+      <c r="G12" s="159" t="s">
         <v>264</v>
       </c>
-      <c r="I12" s="121" t="s">
+      <c r="I12" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="J12" s="119" t="s">
+      <c r="J12" s="156" t="s">
         <v>262</v>
       </c>
-      <c r="K12" s="119"/>
-      <c r="L12" s="119"/>
-      <c r="M12" s="119"/>
-      <c r="N12" s="121" t="s">
+      <c r="K12" s="156"/>
+      <c r="L12" s="156"/>
+      <c r="M12" s="156"/>
+      <c r="N12" s="159" t="s">
         <v>264</v>
       </c>
       <c r="O12" s="48"/>
@@ -12199,7 +12193,7 @@
       </c>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B13" s="121"/>
+      <c r="B13" s="159"/>
       <c r="C13" s="2">
         <v>12</v>
       </c>
@@ -12212,8 +12206,8 @@
       <c r="F13" s="2">
         <v>48</v>
       </c>
-      <c r="G13" s="121"/>
-      <c r="I13" s="121"/>
+      <c r="G13" s="159"/>
+      <c r="I13" s="159"/>
       <c r="J13" s="2">
         <v>12</v>
       </c>
@@ -12226,7 +12220,7 @@
       <c r="M13" s="2">
         <v>48</v>
       </c>
-      <c r="N13" s="121"/>
+      <c r="N13" s="159"/>
       <c r="O13" s="48"/>
       <c r="P13" s="3"/>
     </row>
@@ -12423,14 +12417,14 @@
       <c r="C20" s="77">
         <v>0.05</v>
       </c>
-      <c r="I20" s="119" t="s">
+      <c r="I20" s="156" t="s">
         <v>269</v>
       </c>
-      <c r="J20" s="119"/>
-      <c r="K20" s="119"/>
-      <c r="L20" s="119"/>
-      <c r="M20" s="119"/>
-      <c r="N20" s="119"/>
+      <c r="J20" s="156"/>
+      <c r="K20" s="156"/>
+      <c r="L20" s="156"/>
+      <c r="M20" s="156"/>
+      <c r="N20" s="156"/>
       <c r="O20" s="47"/>
       <c r="P20" s="3" t="s">
         <v>70</v>
@@ -12446,16 +12440,16 @@
       </c>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="I21" s="121" t="s">
+      <c r="I21" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="J21" s="119" t="s">
+      <c r="J21" s="156" t="s">
         <v>262</v>
       </c>
-      <c r="K21" s="119"/>
-      <c r="L21" s="119"/>
-      <c r="M21" s="119"/>
-      <c r="N21" s="121" t="s">
+      <c r="K21" s="156"/>
+      <c r="L21" s="156"/>
+      <c r="M21" s="156"/>
+      <c r="N21" s="159" t="s">
         <v>264</v>
       </c>
       <c r="O21" s="48"/>
@@ -12477,7 +12471,7 @@
       </c>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="I22" s="121"/>
+      <c r="I22" s="159"/>
       <c r="J22" s="2">
         <v>12</v>
       </c>
@@ -12490,7 +12484,7 @@
       <c r="M22" s="2">
         <v>48</v>
       </c>
-      <c r="N22" s="121"/>
+      <c r="N22" s="159"/>
       <c r="O22" s="48"/>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.2">
@@ -12626,13 +12620,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:F12"/>
     <mergeCell ref="I20:N20"/>
     <mergeCell ref="I21:I22"/>
     <mergeCell ref="J21:M21"/>
@@ -12647,6 +12634,13 @@
     <mergeCell ref="I2:M2"/>
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="J3:M3"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>